<commit_message>
tested gradient inversion - bug fix
</commit_message>
<xml_diff>
--- a/RESULT_SUMMARY.xlsx
+++ b/RESULT_SUMMARY.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politoit-my.sharepoint.com/personal/s306089_studenti_polito_it/Documents/PoliTO/MASTER/MACHINE LEARNING AND DEEP LEARNING/FEDERATED LEARNING/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politoit-my.sharepoint.com/personal/s306089_studenti_polito_it/Documents/PoliTO/MASTER/MACHINE LEARNING AND DEEP LEARNING/MLDL Federated Learning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="321" documentId="14_{5D7C720F-F93E-496B-97CE-ECDD9BC9B594}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{762BB7F1-AA54-418E-8B03-8D281C355080}"/>
+  <xr:revisionPtr revIDLastSave="339" documentId="14_{5D7C720F-F93E-496B-97CE-ECDD9BC9B594}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BAC35B26-0568-42DB-8DDD-9A9451090D47}"/>
   <bookViews>
-    <workbookView xWindow="5010" yWindow="3960" windowWidth="28395" windowHeight="18780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8325" yWindow="2205" windowWidth="28395" windowHeight="18780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="19">
   <si>
     <t>NORMALIZATION</t>
   </si>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t>unbalance</t>
+  </si>
+  <si>
+    <t>v2</t>
+  </si>
+  <si>
+    <t>v1</t>
   </si>
 </sst>
 </file>
@@ -131,7 +137,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -154,6 +160,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1025,7 +1032,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>14</v>
       </c>
@@ -1060,48 +1067,48 @@
         <v>12</v>
       </c>
       <c r="L17" s="5">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="7">
+        <v>100</v>
+      </c>
+      <c r="C18" s="7">
+        <v>1E-3</v>
+      </c>
+      <c r="D18" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E18" s="7">
+        <v>5</v>
+      </c>
+      <c r="F18" s="7">
+        <v>1</v>
+      </c>
+      <c r="G18" s="7">
+        <v>1</v>
+      </c>
+      <c r="H18" s="7">
+        <v>0</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J18" s="12">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="K18" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L18" s="8">
         <v>0.67</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="4">
-        <v>100</v>
-      </c>
-      <c r="C18" s="4">
-        <v>1E-3</v>
-      </c>
-      <c r="D18" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="E18" s="4">
-        <v>5</v>
-      </c>
-      <c r="F18" s="4">
-        <v>1</v>
-      </c>
-      <c r="G18" s="4">
-        <v>1</v>
-      </c>
-      <c r="H18" s="4">
-        <v>0</v>
-      </c>
-      <c r="I18" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J18" s="6">
-        <v>5.0000000000000001E-4</v>
-      </c>
-      <c r="K18" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="L18" s="5">
-        <v>0.67</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>14</v>
       </c>
@@ -1139,7 +1146,7 @@
         <v>0.89</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>9</v>
       </c>
@@ -1177,7 +1184,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>14</v>
       </c>
@@ -1215,7 +1222,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -1253,7 +1260,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -1291,7 +1298,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -1329,7 +1336,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>9</v>
       </c>
@@ -1367,7 +1374,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -1404,6 +1411,175 @@
       <c r="L28" s="1">
         <v>0.28999999999999998</v>
       </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31">
+        <v>100</v>
+      </c>
+      <c r="C31">
+        <v>1E-3</v>
+      </c>
+      <c r="D31">
+        <v>0.1</v>
+      </c>
+      <c r="E31">
+        <v>10</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31" t="s">
+        <v>11</v>
+      </c>
+      <c r="J31" s="2">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="K31" t="s">
+        <v>12</v>
+      </c>
+      <c r="L31" s="1">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32">
+        <v>100</v>
+      </c>
+      <c r="C32">
+        <v>1E-3</v>
+      </c>
+      <c r="D32">
+        <v>0.1</v>
+      </c>
+      <c r="E32">
+        <v>10</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32" t="s">
+        <v>11</v>
+      </c>
+      <c r="J32" s="2">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="K32" t="s">
+        <v>12</v>
+      </c>
+      <c r="L32" s="1">
+        <v>0.65</v>
+      </c>
+      <c r="M32">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33">
+        <v>100</v>
+      </c>
+      <c r="C33">
+        <v>1E-3</v>
+      </c>
+      <c r="D33">
+        <v>0.1</v>
+      </c>
+      <c r="E33">
+        <v>10</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33" t="s">
+        <v>11</v>
+      </c>
+      <c r="J33" s="2">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="K33">
+        <v>4</v>
+      </c>
+      <c r="M33">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>9</v>
+      </c>
+      <c r="B34">
+        <v>100</v>
+      </c>
+      <c r="C34">
+        <v>1E-3</v>
+      </c>
+      <c r="D34">
+        <v>0.1</v>
+      </c>
+      <c r="E34">
+        <v>10</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+      <c r="I34" t="s">
+        <v>11</v>
+      </c>
+      <c r="J34" s="2">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="K34">
+        <v>4</v>
+      </c>
+      <c r="M34">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J35" s="2"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J36" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
test with new random seed
</commit_message>
<xml_diff>
--- a/RESULT_SUMMARY.xlsx
+++ b/RESULT_SUMMARY.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politoit-my.sharepoint.com/personal/s306089_studenti_polito_it/Documents/PoliTO/MASTER/MACHINE LEARNING AND DEEP LEARNING/MLDL Federated Learning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="69" documentId="13_ncr:1_{FA094368-407E-439F-8C3E-8492F4A9DC31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B66171E-187A-4FD3-80BA-17301F342636}"/>
+  <xr:revisionPtr revIDLastSave="89" documentId="13_ncr:1_{FA094368-407E-439F-8C3E-8492F4A9DC31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4443CBC6-DE4E-4FA7-82E9-238985CAB747}"/>
   <bookViews>
-    <workbookView xWindow="3135" yWindow="5535" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="22">
   <si>
     <t>NORMALIZATION</t>
   </si>
@@ -95,13 +95,19 @@
   </si>
   <si>
     <t>Ec</t>
+  </si>
+  <si>
+    <t>COMM ROUNDS</t>
+  </si>
+  <si>
+    <t>new seed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,8 +144,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -163,6 +176,11 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -173,11 +191,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -204,9 +223,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -485,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N30" sqref="N30"/>
+    <sheetView tabSelected="1" zoomScale="196" zoomScaleNormal="196" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,7 +527,7 @@
     <col min="12" max="12" width="10.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -540,8 +561,11 @@
       <c r="K1" s="10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P1" s="16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -581,7 +605,7 @@
       <c r="M2" s="7"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -621,7 +645,7 @@
       <c r="M3" s="7"/>
       <c r="N3" s="3"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -637,7 +661,7 @@
       <c r="M4" s="7"/>
       <c r="N4" s="3"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -678,8 +702,11 @@
         <v>0.68</v>
       </c>
       <c r="N5" s="3"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P5" s="16">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -720,8 +747,11 @@
         <v>0.67</v>
       </c>
       <c r="N6" s="3"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P6" s="16">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
@@ -762,8 +792,11 @@
         <v>0.66</v>
       </c>
       <c r="N7" s="3"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P7" s="16">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -804,8 +837,11 @@
         <v>0.42</v>
       </c>
       <c r="N8" s="3"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P8" s="16">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
@@ -846,8 +882,11 @@
         <v>0.46</v>
       </c>
       <c r="N9" s="3"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P9" s="16">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
@@ -888,8 +927,11 @@
         <v>0.45</v>
       </c>
       <c r="N10" s="3"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P10" s="16">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -905,23 +947,23 @@
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="J13" s="2"/>
       <c r="L13" s="9"/>
       <c r="M13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="L14" s="8"/>
       <c r="M14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="L16" s="14"/>
       <c r="M16" t="s">
         <v>17</v>
@@ -932,7 +974,7 @@
         <v>0</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>13</v>
@@ -970,7 +1012,7 @@
         <v>9</v>
       </c>
       <c r="B20" s="3">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="C20" s="3">
         <v>1E-3</v>
@@ -1011,7 +1053,7 @@
         <v>9</v>
       </c>
       <c r="B21" s="3">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="C21" s="3">
         <v>1E-3</v>
@@ -1052,7 +1094,7 @@
         <v>9</v>
       </c>
       <c r="B22" s="3">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="C22" s="3">
         <v>1E-3</v>
@@ -1093,7 +1135,7 @@
         <v>7</v>
       </c>
       <c r="B23" s="3">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="C23" s="3">
         <v>1E-3</v>
@@ -1134,7 +1176,7 @@
         <v>7</v>
       </c>
       <c r="B24" s="3">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="C24" s="3">
         <v>1E-3</v>
@@ -1175,7 +1217,7 @@
         <v>7</v>
       </c>
       <c r="B25" s="3">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="C25" s="3">
         <v>1E-3</v>

</xml_diff>